<commit_message>
AV BD ...... 06Jun2024
</commit_message>
<xml_diff>
--- a/03 Assessments/NOTAS AV - Banco de Dados - 2024.1 Wyden UniRuy.xlsx
+++ b/03 Assessments/NOTAS AV - Banco de Dados - 2024.1 Wyden UniRuy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heleno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\28 WydenArea1BancoDados\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AC5CA8-944D-4620-8338-B40337A6AD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AC6830-14FA-44AB-A687-CE25D00FDF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{413AB662-3705-4BE9-8AD4-FDF0F3F54212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
   <si>
     <t>AV</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>https://youtu.be/CYFaM-U7-mM</t>
+  </si>
+  <si>
+    <t>GitHub - She-Minerva/Banco-de-Dados--PataQuePariu; entrega atrasado e com link quebrado</t>
   </si>
 </sst>
 </file>
@@ -343,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +365,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -556,7 +571,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -617,9 +632,6 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -632,6 +644,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -971,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2841AE5-15C3-4767-A901-0C645FE8FC21}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -987,11 +1008,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="A1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1041,7 +1062,7 @@
       <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -1054,7 +1075,7 @@
         <f t="shared" ref="E4:E34" si="0">C4*0.6+D4</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="7"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1063,7 +1084,7 @@
       <c r="A5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -1076,7 +1097,7 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="7"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1101,7 +1122,7 @@
       <c r="F6" s="7">
         <v>2</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>73</v>
       </c>
       <c r="H6" s="6"/>
@@ -1111,7 +1132,7 @@
       <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="18">
@@ -1124,7 +1145,7 @@
         <f t="shared" si="0"/>
         <v>5.3999999999999995</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="7"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1146,7 +1167,7 @@
         <f t="shared" si="0"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="7"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1168,7 +1189,7 @@
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="7"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1273,7 +1294,7 @@
       <c r="A14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="18" t="s">
@@ -1286,7 +1307,7 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="28"/>
       <c r="G14" s="7"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -1308,7 +1329,7 @@
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="7"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1317,7 +1338,7 @@
       <c r="A16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -1330,7 +1351,7 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="7"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1355,7 +1376,7 @@
       <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="22" t="s">
         <v>72</v>
       </c>
       <c r="H17" s="6"/>
@@ -1405,7 +1426,7 @@
       <c r="F19" s="7">
         <v>4</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="23" t="s">
         <v>75</v>
       </c>
       <c r="H19" s="6"/>
@@ -1463,7 +1484,7 @@
       <c r="A22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="18">
@@ -1476,7 +1497,7 @@
         <f t="shared" si="0"/>
         <v>5.3999999999999995</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="28"/>
       <c r="G22" s="7"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1509,20 +1530,22 @@
       <c r="A24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="27" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="18">
         <v>8</v>
       </c>
       <c r="D24" s="18">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E24" s="19">
         <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="F24" s="7"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F24" s="7">
+        <v>6</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1531,20 +1554,22 @@
       <c r="A25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="9">
         <v>5</v>
       </c>
       <c r="D25" s="18">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E25" s="19">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F25" s="7"/>
+        <v>6.5</v>
+      </c>
+      <c r="F25" s="7">
+        <v>6</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1574,20 +1599,25 @@
       <c r="A27" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="27" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="10">
         <v>7</v>
       </c>
       <c r="D27" s="18">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E27" s="19">
         <f t="shared" si="0"/>
-        <v>4.2</v>
-      </c>
-      <c r="F27" s="7"/>
+        <v>7.7</v>
+      </c>
+      <c r="F27" s="7">
+        <v>6</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
@@ -1609,7 +1639,7 @@
       <c r="F28" s="7">
         <v>3</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="22" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1617,7 +1647,7 @@
       <c r="A29" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C29" s="10" t="s">
@@ -1630,7 +1660,7 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
@@ -1640,14 +1670,14 @@
         <v>45</v>
       </c>
       <c r="C30" s="9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D30" s="18">
         <v>4</v>
       </c>
       <c r="E30" s="19">
         <f t="shared" si="0"/>
-        <v>8.1999999999999993</v>
+        <v>9.3999999999999986</v>
       </c>
       <c r="F30" s="7">
         <v>5</v>
@@ -1657,7 +1687,7 @@
       <c r="A31" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C31" s="10" t="s">
@@ -1670,7 +1700,7 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
@@ -1718,7 +1748,7 @@
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C34" s="15">
@@ -1731,7 +1761,7 @@
         <f t="shared" si="0"/>
         <v>5.3999999999999995</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="28"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1739,52 +1769,52 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="22" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="22" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="22" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="22" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="22" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="22" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1810,6 +1840,7 @@
     <hyperlink ref="A45" r:id="rId12" tooltip="https://youtu.be/cu0_mpuzvgm" xr:uid="{3D284114-EF8D-4B99-9BBC-E6AF64878778}"/>
     <hyperlink ref="A46" r:id="rId13" tooltip="https://youtu.be/hciycjggsfo" xr:uid="{A374E157-BD09-4A69-B985-E65E7237A8A7}"/>
     <hyperlink ref="A47" r:id="rId14" tooltip="https://youtu.be/cyfam-u7-mm" xr:uid="{F7B6ECBF-6F8E-4D37-AD22-65BE39DD4CE8}"/>
+    <hyperlink ref="G27" r:id="rId15" display="https://github.com/She-Minerva/Banco-de-Dados--PataQuePariu" xr:uid="{9BEDD5AF-9758-4F8C-81A0-ED645A5CBC06}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>